<commit_message>
14000618 updated and two weeks emplty places has been filled
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\den\dendataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07250151-1B1D-4BE3-A1E4-E257DA892357}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C129F62-35C4-4ACA-9922-68A2C821A26A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="236">
   <si>
     <t>نرخ خرده فروشی در بازار سنا (ریال)</t>
   </si>
@@ -727,6 +727,12 @@
   </si>
   <si>
     <t>بازار ارز متشکل 17 شهریور سال 1400</t>
+  </si>
+  <si>
+    <t>بازار ارز متشکل و سامانه سنا در 18 شهریور سال 1400</t>
+  </si>
+  <si>
+    <t>بازار ارز متشکل 18 شهریور سال 1400</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1070"/>
+  <dimension ref="A1:J1082"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1049" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1071" sqref="E1071"/>
+    <sheetView tabSelected="1" topLeftCell="A1064" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1079" sqref="F1079"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16949,106 +16955,241 @@
         <v>0.33</v>
       </c>
     </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1074" s="6"/>
+      <c r="B1074" s="6"/>
+      <c r="C1074" s="6"/>
+      <c r="D1074" s="6"/>
+      <c r="E1074" s="6"/>
+      <c r="F1074" s="6"/>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1075" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1075" s="53"/>
+      <c r="C1075" s="53"/>
+      <c r="D1075" s="53"/>
+      <c r="E1075" s="53"/>
+      <c r="F1075" s="53"/>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1076" s="1"/>
+      <c r="B1076" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1076" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1076" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1076" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1076" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" ht="18" x14ac:dyDescent="0.5">
+      <c r="A1077" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1077" s="51">
+        <v>26624</v>
+      </c>
+      <c r="C1077" s="52">
+        <v>26936</v>
+      </c>
+      <c r="D1077">
+        <v>84</v>
+      </c>
+      <c r="E1077" s="52">
+        <v>27820</v>
+      </c>
+      <c r="F1077" s="9">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" ht="18" x14ac:dyDescent="0.5">
+      <c r="A1078" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1078" s="51">
+        <v>31234</v>
+      </c>
+      <c r="C1078" s="52">
+        <v>31623</v>
+      </c>
+      <c r="D1078">
+        <v>93</v>
+      </c>
+      <c r="E1078" s="52">
+        <v>32652</v>
+      </c>
+      <c r="F1078" s="9">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1079" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1079" s="53"/>
+      <c r="C1079" s="53"/>
+      <c r="D1079" s="53"/>
+      <c r="E1079" s="53"/>
+      <c r="F1079" s="50"/>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1080" s="1"/>
+      <c r="B1080" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1080" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1080" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" ht="18" x14ac:dyDescent="0.5">
+      <c r="A1081" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1081" s="51">
+        <v>26589</v>
+      </c>
+      <c r="C1081" s="4">
+        <v>75</v>
+      </c>
+      <c r="D1081" s="51">
+        <v>6494700</v>
+      </c>
+      <c r="E1081" s="5">
+        <v>-0.35</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:6" ht="18" x14ac:dyDescent="0.5">
+      <c r="A1082" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1082" s="51">
+        <v>31217</v>
+      </c>
+      <c r="C1082" s="4">
+        <v>58</v>
+      </c>
+      <c r="D1082" s="51">
+        <v>1009100</v>
+      </c>
+      <c r="E1082" s="5">
+        <v>-0.35</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="218">
-    <mergeCell ref="A1063:F1063"/>
-    <mergeCell ref="A1067:E1067"/>
-    <mergeCell ref="A1040:F1040"/>
-    <mergeCell ref="A1044:E1044"/>
-    <mergeCell ref="A1006:F1006"/>
-    <mergeCell ref="A1010:E1010"/>
-    <mergeCell ref="A982:F982"/>
-    <mergeCell ref="A986:E986"/>
-    <mergeCell ref="A959:F959"/>
-    <mergeCell ref="A963:E963"/>
-    <mergeCell ref="A940:E940"/>
-    <mergeCell ref="A913:F913"/>
-    <mergeCell ref="A917:E917"/>
-    <mergeCell ref="A994:F994"/>
-    <mergeCell ref="A998:E998"/>
-    <mergeCell ref="A891:F891"/>
-    <mergeCell ref="A895:E895"/>
-    <mergeCell ref="A974:E974"/>
-    <mergeCell ref="A936:F936"/>
-    <mergeCell ref="A947:F947"/>
-    <mergeCell ref="A951:E951"/>
-    <mergeCell ref="A925:F925"/>
-    <mergeCell ref="A929:E929"/>
-    <mergeCell ref="A847:F847"/>
-    <mergeCell ref="A851:E851"/>
-    <mergeCell ref="A902:F902"/>
-    <mergeCell ref="A906:E906"/>
-    <mergeCell ref="A803:F803"/>
-    <mergeCell ref="A807:E807"/>
-    <mergeCell ref="A880:F880"/>
-    <mergeCell ref="A884:E884"/>
-    <mergeCell ref="A858:F858"/>
-    <mergeCell ref="A862:E862"/>
-    <mergeCell ref="A836:F836"/>
-    <mergeCell ref="A840:E840"/>
-    <mergeCell ref="A814:F814"/>
-    <mergeCell ref="A818:E818"/>
-    <mergeCell ref="A825:F825"/>
-    <mergeCell ref="A829:E829"/>
-    <mergeCell ref="A869:F869"/>
-    <mergeCell ref="A873:E873"/>
-    <mergeCell ref="A792:F792"/>
-    <mergeCell ref="A796:E796"/>
-    <mergeCell ref="A700:E700"/>
-    <mergeCell ref="A770:F770"/>
-    <mergeCell ref="A774:E774"/>
-    <mergeCell ref="A748:F748"/>
-    <mergeCell ref="A759:F759"/>
-    <mergeCell ref="A763:E763"/>
-    <mergeCell ref="A785:E785"/>
-    <mergeCell ref="A781:F781"/>
-    <mergeCell ref="A752:E752"/>
-    <mergeCell ref="A726:F726"/>
-    <mergeCell ref="A730:E730"/>
-    <mergeCell ref="A706:F706"/>
-    <mergeCell ref="A710:E710"/>
-    <mergeCell ref="A428:E428"/>
-    <mergeCell ref="A487:F487"/>
-    <mergeCell ref="A491:E491"/>
-    <mergeCell ref="A556:F556"/>
-    <mergeCell ref="A560:E560"/>
-    <mergeCell ref="A576:F576"/>
-    <mergeCell ref="A473:E473"/>
-    <mergeCell ref="A433:F433"/>
-    <mergeCell ref="A451:F451"/>
-    <mergeCell ref="A455:E455"/>
-    <mergeCell ref="A549:E549"/>
-    <mergeCell ref="A478:F478"/>
-    <mergeCell ref="A482:E482"/>
-    <mergeCell ref="A496:F496"/>
-    <mergeCell ref="A437:E437"/>
-    <mergeCell ref="A570:E570"/>
-    <mergeCell ref="A446:E446"/>
-    <mergeCell ref="A442:F442"/>
-    <mergeCell ref="A538:E538"/>
-    <mergeCell ref="A545:F545"/>
-    <mergeCell ref="A514:F514"/>
-    <mergeCell ref="A518:E518"/>
-    <mergeCell ref="A534:F534"/>
-    <mergeCell ref="A646:F646"/>
-    <mergeCell ref="A680:E680"/>
-    <mergeCell ref="A686:F686"/>
-    <mergeCell ref="A736:F736"/>
-    <mergeCell ref="A740:E740"/>
-    <mergeCell ref="A640:E640"/>
-    <mergeCell ref="A656:F656"/>
-    <mergeCell ref="A606:F606"/>
-    <mergeCell ref="A610:E610"/>
-    <mergeCell ref="A636:F636"/>
-    <mergeCell ref="A616:F616"/>
-    <mergeCell ref="A620:E620"/>
-    <mergeCell ref="A690:E690"/>
-    <mergeCell ref="A650:E650"/>
-    <mergeCell ref="A676:F676"/>
-    <mergeCell ref="A626:F626"/>
-    <mergeCell ref="A630:E630"/>
-    <mergeCell ref="A716:F716"/>
-    <mergeCell ref="A720:E720"/>
+  <mergeCells count="220">
+    <mergeCell ref="A1075:F1075"/>
+    <mergeCell ref="A1079:E1079"/>
+    <mergeCell ref="A302:E302"/>
+    <mergeCell ref="A325:F325"/>
+    <mergeCell ref="A352:F352"/>
+    <mergeCell ref="A356:E356"/>
+    <mergeCell ref="A1052:F1052"/>
+    <mergeCell ref="A1056:E1056"/>
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A167:E167"/>
+    <mergeCell ref="A136:F136"/>
+    <mergeCell ref="A140:E140"/>
+    <mergeCell ref="A1028:F1028"/>
+    <mergeCell ref="A1032:E1032"/>
+    <mergeCell ref="A1017:F1017"/>
+    <mergeCell ref="A1021:E1021"/>
+    <mergeCell ref="A397:F397"/>
+    <mergeCell ref="A401:E401"/>
+    <mergeCell ref="A253:F253"/>
+    <mergeCell ref="A257:E257"/>
+    <mergeCell ref="A388:F388"/>
+    <mergeCell ref="A415:F415"/>
+    <mergeCell ref="A419:E419"/>
+    <mergeCell ref="A361:F361"/>
+    <mergeCell ref="A970:F970"/>
+    <mergeCell ref="A338:E338"/>
+    <mergeCell ref="A424:F424"/>
+    <mergeCell ref="A307:F307"/>
+    <mergeCell ref="A311:E311"/>
+    <mergeCell ref="A316:F316"/>
+    <mergeCell ref="A320:E320"/>
+    <mergeCell ref="A298:F298"/>
+    <mergeCell ref="A118:F118"/>
+    <mergeCell ref="A122:E122"/>
+    <mergeCell ref="A154:F154"/>
+    <mergeCell ref="A145:F145"/>
+    <mergeCell ref="A149:E149"/>
+    <mergeCell ref="A343:F343"/>
+    <mergeCell ref="A347:E347"/>
+    <mergeCell ref="A383:E383"/>
+    <mergeCell ref="A181:F181"/>
+    <mergeCell ref="A185:E185"/>
+    <mergeCell ref="A235:F235"/>
+    <mergeCell ref="A239:E239"/>
+    <mergeCell ref="A244:F244"/>
+    <mergeCell ref="A190:F190"/>
+    <mergeCell ref="A163:F163"/>
+    <mergeCell ref="A176:E176"/>
+    <mergeCell ref="A158:E158"/>
+    <mergeCell ref="A370:F370"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A113:E113"/>
+    <mergeCell ref="A271:F271"/>
+    <mergeCell ref="A275:E275"/>
+    <mergeCell ref="A266:E266"/>
+    <mergeCell ref="A289:F289"/>
+    <mergeCell ref="A293:E293"/>
+    <mergeCell ref="A334:F334"/>
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A226:F226"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A262:F262"/>
+    <mergeCell ref="A329:E329"/>
+    <mergeCell ref="A280:F280"/>
+    <mergeCell ref="A284:E284"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="A248:E248"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="A203:E203"/>
+    <mergeCell ref="A217:F217"/>
+    <mergeCell ref="A221:E221"/>
+    <mergeCell ref="A208:F208"/>
+    <mergeCell ref="A212:E212"/>
+    <mergeCell ref="A131:E131"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A19:F19"/>
     <mergeCell ref="A374:E374"/>
     <mergeCell ref="A365:E365"/>
     <mergeCell ref="A392:E392"/>
@@ -17073,102 +17214,104 @@
     <mergeCell ref="A500:E500"/>
     <mergeCell ref="A523:F523"/>
     <mergeCell ref="A600:E600"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A113:E113"/>
-    <mergeCell ref="A271:F271"/>
-    <mergeCell ref="A275:E275"/>
-    <mergeCell ref="A266:E266"/>
-    <mergeCell ref="A289:F289"/>
-    <mergeCell ref="A293:E293"/>
-    <mergeCell ref="A334:F334"/>
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A226:F226"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A262:F262"/>
-    <mergeCell ref="A329:E329"/>
-    <mergeCell ref="A280:F280"/>
-    <mergeCell ref="A284:E284"/>
-    <mergeCell ref="A172:F172"/>
-    <mergeCell ref="A248:E248"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="A203:E203"/>
-    <mergeCell ref="A217:F217"/>
-    <mergeCell ref="A221:E221"/>
-    <mergeCell ref="A208:F208"/>
-    <mergeCell ref="A212:E212"/>
-    <mergeCell ref="A131:E131"/>
-    <mergeCell ref="A424:F424"/>
-    <mergeCell ref="A307:F307"/>
-    <mergeCell ref="A311:E311"/>
-    <mergeCell ref="A316:F316"/>
-    <mergeCell ref="A320:E320"/>
-    <mergeCell ref="A298:F298"/>
-    <mergeCell ref="A118:F118"/>
-    <mergeCell ref="A122:E122"/>
-    <mergeCell ref="A154:F154"/>
-    <mergeCell ref="A145:F145"/>
-    <mergeCell ref="A149:E149"/>
-    <mergeCell ref="A343:F343"/>
-    <mergeCell ref="A347:E347"/>
-    <mergeCell ref="A383:E383"/>
-    <mergeCell ref="A181:F181"/>
-    <mergeCell ref="A185:E185"/>
-    <mergeCell ref="A235:F235"/>
-    <mergeCell ref="A239:E239"/>
-    <mergeCell ref="A244:F244"/>
-    <mergeCell ref="A190:F190"/>
-    <mergeCell ref="A163:F163"/>
-    <mergeCell ref="A176:E176"/>
-    <mergeCell ref="A158:E158"/>
-    <mergeCell ref="A370:F370"/>
-    <mergeCell ref="A302:E302"/>
-    <mergeCell ref="A325:F325"/>
-    <mergeCell ref="A352:F352"/>
-    <mergeCell ref="A356:E356"/>
-    <mergeCell ref="A1052:F1052"/>
-    <mergeCell ref="A1056:E1056"/>
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A167:E167"/>
-    <mergeCell ref="A136:F136"/>
-    <mergeCell ref="A140:E140"/>
-    <mergeCell ref="A1028:F1028"/>
-    <mergeCell ref="A1032:E1032"/>
-    <mergeCell ref="A1017:F1017"/>
-    <mergeCell ref="A1021:E1021"/>
-    <mergeCell ref="A397:F397"/>
-    <mergeCell ref="A401:E401"/>
-    <mergeCell ref="A253:F253"/>
-    <mergeCell ref="A257:E257"/>
-    <mergeCell ref="A388:F388"/>
-    <mergeCell ref="A415:F415"/>
-    <mergeCell ref="A419:E419"/>
-    <mergeCell ref="A361:F361"/>
-    <mergeCell ref="A970:F970"/>
-    <mergeCell ref="A338:E338"/>
+    <mergeCell ref="A646:F646"/>
+    <mergeCell ref="A680:E680"/>
+    <mergeCell ref="A686:F686"/>
+    <mergeCell ref="A736:F736"/>
+    <mergeCell ref="A740:E740"/>
+    <mergeCell ref="A640:E640"/>
+    <mergeCell ref="A656:F656"/>
+    <mergeCell ref="A606:F606"/>
+    <mergeCell ref="A610:E610"/>
+    <mergeCell ref="A636:F636"/>
+    <mergeCell ref="A616:F616"/>
+    <mergeCell ref="A620:E620"/>
+    <mergeCell ref="A690:E690"/>
+    <mergeCell ref="A650:E650"/>
+    <mergeCell ref="A676:F676"/>
+    <mergeCell ref="A626:F626"/>
+    <mergeCell ref="A630:E630"/>
+    <mergeCell ref="A716:F716"/>
+    <mergeCell ref="A720:E720"/>
+    <mergeCell ref="A428:E428"/>
+    <mergeCell ref="A487:F487"/>
+    <mergeCell ref="A491:E491"/>
+    <mergeCell ref="A556:F556"/>
+    <mergeCell ref="A560:E560"/>
+    <mergeCell ref="A576:F576"/>
+    <mergeCell ref="A473:E473"/>
+    <mergeCell ref="A433:F433"/>
+    <mergeCell ref="A451:F451"/>
+    <mergeCell ref="A455:E455"/>
+    <mergeCell ref="A549:E549"/>
+    <mergeCell ref="A478:F478"/>
+    <mergeCell ref="A482:E482"/>
+    <mergeCell ref="A496:F496"/>
+    <mergeCell ref="A437:E437"/>
+    <mergeCell ref="A570:E570"/>
+    <mergeCell ref="A446:E446"/>
+    <mergeCell ref="A442:F442"/>
+    <mergeCell ref="A538:E538"/>
+    <mergeCell ref="A545:F545"/>
+    <mergeCell ref="A514:F514"/>
+    <mergeCell ref="A518:E518"/>
+    <mergeCell ref="A534:F534"/>
+    <mergeCell ref="A792:F792"/>
+    <mergeCell ref="A796:E796"/>
+    <mergeCell ref="A700:E700"/>
+    <mergeCell ref="A770:F770"/>
+    <mergeCell ref="A774:E774"/>
+    <mergeCell ref="A748:F748"/>
+    <mergeCell ref="A759:F759"/>
+    <mergeCell ref="A763:E763"/>
+    <mergeCell ref="A785:E785"/>
+    <mergeCell ref="A781:F781"/>
+    <mergeCell ref="A752:E752"/>
+    <mergeCell ref="A726:F726"/>
+    <mergeCell ref="A730:E730"/>
+    <mergeCell ref="A706:F706"/>
+    <mergeCell ref="A710:E710"/>
+    <mergeCell ref="A847:F847"/>
+    <mergeCell ref="A851:E851"/>
+    <mergeCell ref="A902:F902"/>
+    <mergeCell ref="A906:E906"/>
+    <mergeCell ref="A803:F803"/>
+    <mergeCell ref="A807:E807"/>
+    <mergeCell ref="A880:F880"/>
+    <mergeCell ref="A884:E884"/>
+    <mergeCell ref="A858:F858"/>
+    <mergeCell ref="A862:E862"/>
+    <mergeCell ref="A836:F836"/>
+    <mergeCell ref="A840:E840"/>
+    <mergeCell ref="A814:F814"/>
+    <mergeCell ref="A818:E818"/>
+    <mergeCell ref="A825:F825"/>
+    <mergeCell ref="A829:E829"/>
+    <mergeCell ref="A869:F869"/>
+    <mergeCell ref="A873:E873"/>
+    <mergeCell ref="A940:E940"/>
+    <mergeCell ref="A913:F913"/>
+    <mergeCell ref="A917:E917"/>
+    <mergeCell ref="A994:F994"/>
+    <mergeCell ref="A998:E998"/>
+    <mergeCell ref="A891:F891"/>
+    <mergeCell ref="A895:E895"/>
+    <mergeCell ref="A974:E974"/>
+    <mergeCell ref="A936:F936"/>
+    <mergeCell ref="A947:F947"/>
+    <mergeCell ref="A951:E951"/>
+    <mergeCell ref="A925:F925"/>
+    <mergeCell ref="A929:E929"/>
+    <mergeCell ref="A1063:F1063"/>
+    <mergeCell ref="A1067:E1067"/>
+    <mergeCell ref="A1040:F1040"/>
+    <mergeCell ref="A1044:E1044"/>
+    <mergeCell ref="A1006:F1006"/>
+    <mergeCell ref="A1010:E1010"/>
+    <mergeCell ref="A982:F982"/>
+    <mergeCell ref="A986:E986"/>
+    <mergeCell ref="A959:F959"/>
+    <mergeCell ref="A963:E963"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>